<commit_message>
goals overview and february adaptations
</commit_message>
<xml_diff>
--- a/data/Firmen/creators/2025-01-01/Daily_Scores.xlsx
+++ b/data/Firmen/creators/2025-01-01/Daily_Scores.xlsx
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>9.172867264528152</v>
+        <v>9.067686116209028</v>
       </c>
       <c r="D82" t="n">
         <v>10</v>
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>19.17286726452815</v>
+        <v>19.06768611620903</v>
       </c>
     </row>
     <row r="83">

</xml_diff>